<commit_message>
Updated mean summary results
</commit_message>
<xml_diff>
--- a/results/summary-means/mean_accel_diel_period_hab.xlsx
+++ b/results/summary-means/mean_accel_diel_period_hab.xlsx
@@ -496,14 +496,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7"/>
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" t="n">
-        <v>0.56</v>
+        <v>0.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.074</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="8">
@@ -514,13 +516,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="E8" t="n">
-        <v>0.009</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="9">
@@ -531,13 +533,13 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
-        <v>0.95</v>
+        <v>0.87</v>
       </c>
       <c r="E9" t="n">
-        <v>0.063</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="10">
@@ -548,13 +550,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>0.87</v>
+        <v>0.37</v>
       </c>
       <c r="E10" t="n">
-        <v>0.053</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="11">
@@ -565,13 +567,13 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>0.37</v>
+        <v>0.49</v>
       </c>
       <c r="E11" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="12">
@@ -579,16 +581,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>0.49</v>
       </c>
       <c r="E12" t="n">
-        <v>0.007</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="13">
@@ -596,14 +598,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13"/>
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
       <c r="D13" t="n">
-        <v>0.83</v>
+        <v>0.43</v>
       </c>
       <c r="E13" t="n">
-        <v>0.038</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="14">
@@ -614,13 +618,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>0.49</v>
+        <v>0.77</v>
       </c>
       <c r="E14" t="n">
-        <v>0.026</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="15">
@@ -631,13 +635,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
-        <v>0.43</v>
+        <v>0.41</v>
       </c>
       <c r="E15" t="n">
-        <v>0.239</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="16">
@@ -648,13 +652,13 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>0.77</v>
+        <v>0.5</v>
       </c>
       <c r="E16" t="n">
-        <v>0.137</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="17">
@@ -662,16 +666,16 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
-        <v>0.41</v>
+        <v>0.28</v>
       </c>
       <c r="E17" t="n">
-        <v>0.026</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="18">
@@ -679,16 +683,16 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E18" t="n">
-        <v>0.024</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="19">
@@ -696,14 +700,16 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19"/>
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
       <c r="D19" t="n">
-        <v>0.32</v>
+        <v>0.71</v>
       </c>
       <c r="E19" t="n">
-        <v>0.113</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="20">
@@ -714,13 +720,13 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="E20" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="21">
@@ -731,79 +737,81 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6</v>
+        <v>0.31</v>
       </c>
       <c r="E21" t="n">
-        <v>0.042</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" t="n">
-        <v>0.71</v>
+        <v>0.17</v>
       </c>
       <c r="E22" t="n">
-        <v>0.073</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="E23" t="n">
-        <v>0.007</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" t="n">
-        <v>0.31</v>
+        <v>0.18</v>
       </c>
       <c r="E24" t="n">
-        <v>0.005</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25"/>
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
       <c r="D25" t="n">
-        <v>0.39</v>
+        <v>0.18</v>
       </c>
       <c r="E25" t="n">
-        <v>0.033</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="26">
@@ -814,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="E26" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="27">
@@ -828,16 +836,16 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
-        <v>0.26</v>
+        <v>0.15</v>
       </c>
       <c r="E27" t="n">
-        <v>0.028</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="28">
@@ -845,13 +853,13 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="E28" t="n">
         <v>0.008</v>
@@ -862,16 +870,16 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="E29" t="n">
-        <v>0.011</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="30">
@@ -879,16 +887,16 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
         <v>0.2</v>
       </c>
       <c r="E30" t="n">
-        <v>0.006</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="31">
@@ -896,14 +904,16 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31"/>
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
       <c r="D31" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="E31" t="n">
-        <v>0.008</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="32">
@@ -911,16 +921,16 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="E32" t="n">
-        <v>0.001</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="33">
@@ -928,16 +938,16 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>0.19</v>
+        <v>0.29</v>
       </c>
       <c r="E33" t="n">
-        <v>0.008</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="34">
@@ -945,16 +955,16 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="n">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="E34" t="n">
-        <v>0.002</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="35">
@@ -962,16 +972,16 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
         <v>10</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E35" t="n">
-        <v>0.004</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="36">
@@ -979,16 +989,16 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="n">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
       <c r="E36" t="n">
-        <v>0.002</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="37">
@@ -996,14 +1006,16 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37"/>
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
       <c r="D37" t="n">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="E37" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="38">
@@ -1011,16 +1023,16 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="E38" t="n">
-        <v>0.004</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="39">
@@ -1028,16 +1040,16 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="E39" t="n">
-        <v>0.026</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="40">
@@ -1045,16 +1057,16 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" t="n">
-        <v>0.24</v>
+        <v>0.14</v>
       </c>
       <c r="E40" t="n">
-        <v>0.009</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="41">
@@ -1062,148 +1074,16 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3</v>
+        <v>0.14</v>
       </c>
       <c r="E41" t="n">
-        <v>0.022</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.007</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43"/>
-      <c r="D43" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.011</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.009</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.003</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.004</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="E48" t="n">
         <v>0.002</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49"/>
-      <c r="D49" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>